<commit_message>
Modificamos la practica 2 del bloque 4
</commit_message>
<xml_diff>
--- a/Practicas/Bloque4/Bloque4_2/Reporte_Ejecutivo_COO.xlsx
+++ b/Practicas/Bloque4/Bloque4_2/Reporte_Ejecutivo_COO.xlsx
@@ -7,28 +7,21 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="horas" sheetId="1" r:id="rId1"/>
-    <sheet name="días_semana" sheetId="2" r:id="rId2"/>
-    <sheet name="meses" sheetId="3" r:id="rId3"/>
-    <sheet name="tipos_de_pizza" sheetId="4" r:id="rId4"/>
+    <sheet name="reporte_ejecutivo_ventas" sheetId="1" r:id="rId1"/>
+    <sheet name="reporte_de_ingredientes" sheetId="2" r:id="rId2"/>
+    <sheet name="reporte_de_pedidos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'días_semana'!$B$5:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">horas!$B$5:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">meses!$B$5:$C$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'tipos_de_pizza'!$B$5:$C$5</definedName>
-  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="139">
   <si>
     <t>Catalina Royo-Villanova Seguí</t>
   </si>
   <si>
-    <t>REPORTE EVECUTIVO VENTAS MAVEN'S PIZZA</t>
+    <t>REPORTE EJECUTIVO VENTAS DE MAVEN'S PIZZA</t>
   </si>
   <si>
     <t>Pizzas vendidas por hora</t>
@@ -109,6 +102,216 @@
     <t>December</t>
   </si>
   <si>
+    <t>REPORTE DE INGREDIENTES DE MAVEN'S PIZZA</t>
+  </si>
+  <si>
+    <t>Ingredientes más y menos usados</t>
+  </si>
+  <si>
+    <t>Ingredient</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Barbecued Chicken</t>
+  </si>
+  <si>
+    <t>Red Peppers</t>
+  </si>
+  <si>
+    <t>Green Peppers</t>
+  </si>
+  <si>
+    <t>Tomatoes</t>
+  </si>
+  <si>
+    <t>Red Onions</t>
+  </si>
+  <si>
+    <t>Barbecue Sauce</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Artichoke</t>
+  </si>
+  <si>
+    <t>Spinach</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Jalapeno Peppers</t>
+  </si>
+  <si>
+    <t>Fontina Cheese</t>
+  </si>
+  <si>
+    <t>Gouda Cheese</t>
+  </si>
+  <si>
+    <t>Mushrooms</t>
+  </si>
+  <si>
+    <t>Asiago Cheese</t>
+  </si>
+  <si>
+    <t>Alfredo Sauce</t>
+  </si>
+  <si>
+    <t>Pesto Sauce</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Cilantro</t>
+  </si>
+  <si>
+    <t>Chipotle Sauce</t>
+  </si>
+  <si>
+    <t>Pineapple</t>
+  </si>
+  <si>
+    <t>Thai Sweet Chilli Sauce</t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>Pepperoni</t>
+  </si>
+  <si>
+    <t>Italian Sausage</t>
+  </si>
+  <si>
+    <t>Chorizo Sausage</t>
+  </si>
+  <si>
+    <t>Sliced Ham</t>
+  </si>
+  <si>
+    <t>Mozzarella Cheese</t>
+  </si>
+  <si>
+    <t>Capocollo</t>
+  </si>
+  <si>
+    <t>Goat Cheese</t>
+  </si>
+  <si>
+    <t>Oregano</t>
+  </si>
+  <si>
+    <t>Anchovies</t>
+  </si>
+  <si>
+    <t>Green Olives</t>
+  </si>
+  <si>
+    <t>Kalamata Olives</t>
+  </si>
+  <si>
+    <t>Feta Cheese</t>
+  </si>
+  <si>
+    <t>Beef Chuck Roast</t>
+  </si>
+  <si>
+    <t>Brie Carre Cheese</t>
+  </si>
+  <si>
+    <t>Prosciutto</t>
+  </si>
+  <si>
+    <t>Caramelized Onions</t>
+  </si>
+  <si>
+    <t>Pears</t>
+  </si>
+  <si>
+    <t>Thyme</t>
+  </si>
+  <si>
+    <t>Nduja Salami</t>
+  </si>
+  <si>
+    <t>Pancetta</t>
+  </si>
+  <si>
+    <t>Friggitello Peppers</t>
+  </si>
+  <si>
+    <t>Calabrese Salami</t>
+  </si>
+  <si>
+    <t>Genoa Salami</t>
+  </si>
+  <si>
+    <t>Prosciutto di San Daniele</t>
+  </si>
+  <si>
+    <t>Arugula</t>
+  </si>
+  <si>
+    <t>Coarse Sicilian Salami</t>
+  </si>
+  <si>
+    <t>Luganega Sausage</t>
+  </si>
+  <si>
+    <t>Onions</t>
+  </si>
+  <si>
+    <t>Soppressata Salami</t>
+  </si>
+  <si>
+    <t>Artichokes</t>
+  </si>
+  <si>
+    <t>Peperoncini verdi</t>
+  </si>
+  <si>
+    <t>Provolone Cheese</t>
+  </si>
+  <si>
+    <t>Smoked Gouda Cheese</t>
+  </si>
+  <si>
+    <t>Romano Cheese</t>
+  </si>
+  <si>
+    <t>Blue Cheese</t>
+  </si>
+  <si>
+    <t>Ricotta Cheese</t>
+  </si>
+  <si>
+    <t>Gorgonzola Piccante Cheese</t>
+  </si>
+  <si>
+    <t>Parmigiano Reggiano Cheese</t>
+  </si>
+  <si>
+    <t>Eggplant</t>
+  </si>
+  <si>
+    <t>Zucchini</t>
+  </si>
+  <si>
+    <t>Sun-dried Tomatoes</t>
+  </si>
+  <si>
+    <t>Plum Tomatoes</t>
+  </si>
+  <si>
+    <t>REPORTE DE PEDIDOS DE MAVEN'S PIZZA</t>
+  </si>
+  <si>
     <t>Tipos de pizzas más y menos vendidos</t>
   </si>
   <si>
@@ -209,6 +412,27 @@
   </si>
   <si>
     <t>brie_carre</t>
+  </si>
+  <si>
+    <t>Tamaños de pizzas más y menos vendidos</t>
+  </si>
+  <si>
+    <t>tamanos</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>xl</t>
+  </si>
+  <si>
+    <t>xxl</t>
   </si>
 </sst>
 </file>
@@ -361,7 +585,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>horas!$B$6:$B$29</c:f>
+              <c:f>reporte_ejecutivo_ventas!$B$6:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -442,7 +666,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>horas!$C$6:$C$29</c:f>
+              <c:f>reporte_ejecutivo_ventas!$C$6:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -542,7 +766,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Hora</a:t>
+                  <a:t>Horas</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -613,7 +837,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>días_semana!$B$6:$B$12</c:f>
+              <c:f>reporte_ejecutivo_ventas!$B$39:$B$45</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -642,7 +866,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>días_semana!$C$6:$C$12</c:f>
+              <c:f>reporte_ejecutivo_ventas!$C$39:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -761,7 +985,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>meses!$B$6:$B$17</c:f>
+              <c:f>reporte_ejecutivo_ventas!$B$72:$B$83</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -805,7 +1029,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>meses!$C$6:$C$17</c:f>
+              <c:f>reporte_ejecutivo_ventas!$C$72:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -869,7 +1093,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Mes</a:t>
+                  <a:t>Año</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -939,7 +1163,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>tipos_de_pizza!$B$6:$B$37</c:f>
+              <c:f>reporte_de_pedidos!$B$6:$B$37</c:f>
               <c:strCache>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
@@ -1043,7 +1267,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>tipos_de_pizza!$C$6:$C$37</c:f>
+              <c:f>reporte_de_pedidos!$C$6:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1167,7 +1391,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Tipos</a:t>
+                  <a:t>tipos</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1223,20 +1447,156 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>reporte_de_pedidos!$B$43:$B$47</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>m</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>l</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>xl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>xxl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>reporte_de_pedidos!$C$43:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16727</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50050001"/>
+        <c:axId val="50050002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50050001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>tamaños</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50050002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nº de ventas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1255,23 +1615,126 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2833</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>106964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="ingredientes_usados.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2447925" y="771525"/>
+          <a:ext cx="6698908" cy="12479939"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1290,27 +1753,22 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1319,42 +1777,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1648,18 +2071,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:O83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:15">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1671,8 +2094,13 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1684,8 +2112,13 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1693,7 +2126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:15">
       <c r="B6" s="4">
         <v>0</v>
       </c>
@@ -1701,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:15">
       <c r="B7" s="4">
         <v>1</v>
       </c>
@@ -1709,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:15">
       <c r="B8" s="4">
         <v>2</v>
       </c>
@@ -1717,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:15">
       <c r="B9" s="4">
         <v>3</v>
       </c>
@@ -1725,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:15">
       <c r="B10" s="4">
         <v>4</v>
       </c>
@@ -1733,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:15">
       <c r="B11" s="4">
         <v>5</v>
       </c>
@@ -1741,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:15">
       <c r="B12" s="4">
         <v>6</v>
       </c>
@@ -1749,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:15">
       <c r="B13" s="4">
         <v>7</v>
       </c>
@@ -1757,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:15">
       <c r="B14" s="4">
         <v>8</v>
       </c>
@@ -1765,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:15">
       <c r="B15" s="4">
         <v>9</v>
       </c>
@@ -1773,7 +2206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:15">
       <c r="B16" s="4">
         <v>10</v>
       </c>
@@ -1885,12 +2318,217 @@
         <v>50</v>
       </c>
     </row>
+    <row r="36" spans="2:15">
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="5">
+        <v>6373</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
+      <c r="B40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="4">
+        <v>5367</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15">
+      <c r="B41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="4">
+        <v>5818</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15">
+      <c r="B42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="4">
+        <v>6099</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="B43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="5">
+        <v>6280</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="5">
+        <v>6689</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="5">
+        <v>7103</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15">
+      <c r="B69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+    </row>
+    <row r="71" spans="2:15">
+      <c r="B71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="2:15">
+      <c r="B72" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="5">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="73" spans="2:15">
+      <c r="B73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="4">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="74" spans="2:15">
+      <c r="B74" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="5">
+        <v>3771</v>
+      </c>
+    </row>
+    <row r="75" spans="2:15">
+      <c r="B75" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="5">
+        <v>3658</v>
+      </c>
+    </row>
+    <row r="76" spans="2:15">
+      <c r="B76" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="5">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="77" spans="2:15">
+      <c r="B77" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C77" s="4">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="78" spans="2:15">
+      <c r="B78" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="5">
+        <v>3883</v>
+      </c>
+    </row>
+    <row r="79" spans="2:15">
+      <c r="B79" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" s="5">
+        <v>3682</v>
+      </c>
+    </row>
+    <row r="80" spans="2:15">
+      <c r="B80" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" s="4">
+        <v>3409</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="4">
+        <v>3439</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82" s="5">
+        <v>3761</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83" s="4">
+        <v>3454</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B5:C5"/>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B36:O36"/>
+    <mergeCell ref="B69:O69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1899,20 +2537,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:15">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1922,10 +2560,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1935,77 +2578,1272 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5">
-        <v>6373</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4">
-        <v>5367</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4">
-        <v>5818</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4">
-        <v>6099</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>31</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4668</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5">
+        <v>31048</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5">
+        <v>9496</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5">
+        <v>51245</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C10" s="5">
-        <v>6280</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="5">
-        <v>6689</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>37206</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4668</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5">
-        <v>7103</v>
-      </c>
+        <v>16722</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4387</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5">
+        <v>17368</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="5">
+        <v>53683</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="B16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="5">
+        <v>11422</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="4">
+        <v>6140</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4387</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="5">
+        <v>16082</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="4">
+        <v>6216</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1804</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="4">
+        <v>4944</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="4">
+        <v>7035</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="4">
+        <v>7035</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="4">
+        <v>7035</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="5">
+        <v>8900</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="4">
+        <v>4837</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="4">
+        <v>5547</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="5">
+        <v>16334</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1633</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1633</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="B32" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="4">
+        <v>4063</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="2:15">
+      <c r="B33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="5">
+        <v>20578</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="2:15">
+      <c r="B34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="5">
+        <v>13295</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" spans="2:15">
+      <c r="B35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="4">
+        <v>6736</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+    </row>
+    <row r="36" spans="2:15">
+      <c r="B36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2809</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+    </row>
+    <row r="37" spans="2:15">
+      <c r="B37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2571</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="B38" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="5">
+        <v>10814</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="4">
+        <v>6632</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+    </row>
+    <row r="40" spans="2:15">
+      <c r="B40" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="5">
+        <v>8873</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" spans="2:15">
+      <c r="B41" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="4">
+        <v>3388</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+    </row>
+    <row r="42" spans="2:15">
+      <c r="B42" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="4">
+        <v>418</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="B43" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="4">
+        <v>418</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="4">
+        <v>418</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="4">
+        <v>418</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+    </row>
+    <row r="46" spans="2:15">
+      <c r="B46" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="4">
+        <v>418</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+    </row>
+    <row r="47" spans="2:15">
+      <c r="B47" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1820</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+    </row>
+    <row r="48" spans="2:15">
+      <c r="B48" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1820</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="B49" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1820</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="4">
+        <v>3689</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+    </row>
+    <row r="51" spans="2:15">
+      <c r="B51" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="4">
+        <v>2870</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+    </row>
+    <row r="52" spans="2:15">
+      <c r="B52" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="4">
+        <v>2535</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="B53" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="4">
+        <v>2535</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+    </row>
+    <row r="54" spans="2:15">
+      <c r="B54" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" s="4">
+        <v>3253</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+    </row>
+    <row r="55" spans="2:15">
+      <c r="B55" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="4">
+        <v>3253</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+    </row>
+    <row r="56" spans="2:15">
+      <c r="B56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="4">
+        <v>3253</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+    </row>
+    <row r="57" spans="2:15">
+      <c r="B57" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1753</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="B58" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="5">
+        <v>10306</v>
+      </c>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+    </row>
+    <row r="59" spans="2:15">
+      <c r="B59" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="4">
+        <v>3927</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+    </row>
+    <row r="60" spans="2:15">
+      <c r="B60" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="4">
+        <v>3684</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+    </row>
+    <row r="61" spans="2:15">
+      <c r="B61" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="4">
+        <v>3684</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="B62" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C62" s="4">
+        <v>3684</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+    </row>
+    <row r="63" spans="2:15">
+      <c r="B63" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" s="4">
+        <v>3684</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+    </row>
+    <row r="64" spans="2:15">
+      <c r="B64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" s="4">
+        <v>4405</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="5"/>
+    </row>
+    <row r="65" spans="2:15">
+      <c r="B65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="4">
+        <v>4405</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
+    </row>
+    <row r="66" spans="2:15">
+      <c r="B66" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" s="4">
+        <v>4405</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+    </row>
+    <row r="67" spans="2:15">
+      <c r="B67" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" s="4">
+        <v>1581</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+    </row>
+    <row r="68" spans="2:15">
+      <c r="B68" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="4">
+        <v>4172</v>
+      </c>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+    </row>
+    <row r="69" spans="2:15">
+      <c r="B69" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" s="4">
+        <v>3256</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="5"/>
+    </row>
+    <row r="70" spans="2:15">
+      <c r="B70" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="4">
+        <v>1702</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:C5"/>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="E5:O70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2014,20 +3852,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:15">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2037,10 +3875,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2050,253 +3893,103 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:15">
       <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5">
-        <v>3730</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3487</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5">
-        <v>3771</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="5">
-        <v>3658</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3828</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4">
-        <v>3627</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5">
-        <v>3883</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="5">
-        <v>3682</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3409</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="4">
-        <v>3439</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="5">
-        <v>3761</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="4">
-        <v>3454</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="B5:C5"/>
-  <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C6" s="5">
         <v>2156</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:15">
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="C7" s="5">
         <v>2152</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:15">
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="C8" s="5">
         <v>2141</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:15">
       <c r="B9" s="5" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="C9" s="5">
         <v>2129</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:15">
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="C10" s="5">
         <v>2071</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:15">
       <c r="B11" s="5" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="C11" s="5">
         <v>2057</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:15">
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C12" s="5">
         <v>1722</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:15">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="C13" s="5">
         <v>1702</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:15">
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="C14" s="5">
         <v>1694</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:15">
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="C15" s="5">
         <v>1687</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:15">
       <c r="B16" s="5" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="C16" s="5">
         <v>1676</v>
@@ -2304,7 +3997,7 @@
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="5" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="C17" s="5">
         <v>1650</v>
@@ -2312,7 +4005,7 @@
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="4" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="C18" s="4">
         <v>1357</v>
@@ -2320,7 +4013,7 @@
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="C19" s="4">
         <v>1302</v>
@@ -2328,7 +4021,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C20" s="4">
         <v>1290</v>
@@ -2336,7 +4029,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="4" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="C21" s="4">
         <v>1290</v>
@@ -2344,7 +4037,7 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="4" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
       <c r="C22" s="4">
         <v>1278</v>
@@ -2352,7 +4045,7 @@
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="4" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="C23" s="4">
         <v>1254</v>
@@ -2360,7 +4053,7 @@
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="4" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="C24" s="4">
         <v>1253</v>
@@ -2368,7 +4061,7 @@
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="4" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="C25" s="4">
         <v>1252</v>
@@ -2376,7 +4069,7 @@
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="4" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C26" s="4">
         <v>1240</v>
@@ -2384,7 +4077,7 @@
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="4" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="C27" s="4">
         <v>1228</v>
@@ -2392,7 +4085,7 @@
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="4" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="C28" s="4">
         <v>884</v>
@@ -2400,7 +4093,7 @@
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="C29" s="4">
         <v>882</v>
@@ -2408,7 +4101,7 @@
     </row>
     <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>124</v>
       </c>
       <c r="C30" s="4">
         <v>876</v>
@@ -2416,7 +4109,7 @@
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="4" t="s">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="C31" s="4">
         <v>860</v>
@@ -2424,58 +4117,124 @@
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="4" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="C32" s="4">
         <v>854</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:15">
       <c r="B33" s="4" t="s">
-        <v>57</v>
+        <v>127</v>
       </c>
       <c r="C33" s="4">
         <v>848</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:15">
       <c r="B34" s="4" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="C34" s="4">
         <v>847</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:15">
       <c r="B35" s="4" t="s">
-        <v>59</v>
+        <v>129</v>
       </c>
       <c r="C35" s="4">
         <v>839</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:15">
       <c r="B36" s="4" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="C36" s="4">
         <v>834</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:15">
       <c r="B37" s="4" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="C37" s="4">
         <v>424</v>
       </c>
     </row>
+    <row r="40" spans="2:15">
+      <c r="B40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+    </row>
+    <row r="42" spans="2:15">
+      <c r="B42" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
+      <c r="B43" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="5">
+        <v>12701</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="5">
+        <v>13802</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="5">
+        <v>16727</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
+      <c r="B46" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="4">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
+      <c r="B47" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" s="4">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B5:C5"/>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B40:O40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>